<commit_message>
added file upload feature
</commit_message>
<xml_diff>
--- a/dyuthi16_schedule.xlsx
+++ b/dyuthi16_schedule.xlsx
@@ -1560,8 +1560,8 @@
   </sheetPr>
   <dimension ref="A1:H185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D162" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G178" activeCellId="0" sqref="G178:G185"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D165" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H186" activeCellId="0" sqref="H186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>